<commit_message>
Corrected GPS coordinates for nest 18.
</commit_message>
<xml_diff>
--- a/data/mod_field_data.xlsx
+++ b/data/mod_field_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mtaylor/Documents/r/paige/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mtaylor/Documents/r/rhyne/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ED374F8-F7FB-6140-B2B3-5ECDDABAEFE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61D3B784-5E67-0D4E-8849-DC4C3F3E446D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25820" windowHeight="15500" xr2:uid="{DB384781-E84E-40A3-9DF6-FD19CA0B4AD2}"/>
   </bookViews>
@@ -822,8 +822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1A5D373-BE8D-41A8-9190-595E23E37102}">
   <dimension ref="A1:N49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C42" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="F5" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1615,10 +1615,10 @@
         <v>31</v>
       </c>
       <c r="M19">
-        <v>37.079120000000003</v>
+        <v>37.131900000000002</v>
       </c>
       <c r="N19">
-        <v>-89.276520000000005</v>
+        <v>-89.460099999999997</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>